<commit_message>
2x camera real world fade mangler implementering
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/ExcelFiles/Categories.xlsx
+++ b/Assets/StreamingAssets/ExcelFiles/Categories.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17870"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>hus</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>transport</t>
+  </si>
+  <si>
+    <t>audi</t>
+  </si>
+  <si>
+    <t>ase</t>
+  </si>
+  <si>
+    <t>ida</t>
+  </si>
+  <si>
+    <t>skat</t>
   </si>
 </sst>
 </file>
@@ -450,15 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:B19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,146 +480,152 @@
       <c r="C1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
jeg har også en kage til dig
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/ExcelFiles/Categories.xlsx
+++ b/Assets/StreamingAssets/ExcelFiles/Categories.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17870"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>hus</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>skat</t>
+  </si>
+  <si>
+    <t>ko</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,6 +631,11 @@
         <v>26</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
IKONER FIX + EXCEL CATEGORIES ARKET
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/ExcelFiles/Categories.xlsx
+++ b/Assets/StreamingAssets/ExcelFiles/Categories.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>hus</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>ko</t>
+  </si>
+  <si>
+    <t>streaming</t>
   </si>
 </sst>
 </file>
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,49 +593,50 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
         <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>